<commit_message>
Finished transfer line class plus test script
</commit_message>
<xml_diff>
--- a/11-Parameters/nuSTORM-TrfLine-Params-v1.0.xlsx
+++ b/11-Parameters/nuSTORM-TrfLine-Params-v1.0.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Momentum acceptance</t>
   </si>
   <si>
-    <t xml:space="preserve">pAcc</t>
+    <t xml:space="preserve">piAcc</t>
   </si>
   <si>
     <t xml:space="preserve">%</t>
@@ -195,7 +195,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,7 +249,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>11</v>

</xml_diff>